<commit_message>
Copmile v5-b21. Update testing files, docs
</commit_message>
<xml_diff>
--- a/deploy/docs/Estimate_WoodBio.xlsx
+++ b/deploy/docs/Estimate_WoodBio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BRM\LANDIS_II\GitCode\aruzicka555\Extension-PnET-Succession\deploy\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1A871F-2A69-49B7-B38E-67CA8DE7547F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BF31FF-817A-41E8-95A1-7C748789C9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30135" yWindow="-11655" windowWidth="14175" windowHeight="11325" xr2:uid="{E2F93AC3-C803-4B76-8EED-92391C83CE40}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E2F93AC3-C803-4B76-8EED-92391C83CE40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="43">
   <si>
     <t>Input WoodBio</t>
   </si>
@@ -144,11 +144,35 @@
   <si>
     <t>pinustro</t>
   </si>
+  <si>
+    <t>WhiteCedar</t>
+  </si>
+  <si>
+    <t>BalsamFir</t>
+  </si>
+  <si>
+    <t>BlackAsh</t>
+  </si>
+  <si>
+    <t>RedMaple</t>
+  </si>
+  <si>
+    <t>NPInOak</t>
+  </si>
+  <si>
+    <t>tiliamer</t>
+  </si>
+  <si>
+    <t>thujocci</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -184,10 +208,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1673,6 +1698,411 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000D-052C-405D-BC33-E3CC430F67BA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:v>WhiteCedar</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.0996171131000249E-2"/>
+                  <c:y val="-8.8274974888020122E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$65:$A$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$65:$B$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6778</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4133</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5449</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3444</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-D8F9-4031-9B78-DEFE5AA57454}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:v>tiliamer</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.25666488551403921"/>
+                  <c:y val="-0.13246135781084056"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$66:$G$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$66:$H$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6095</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4139</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5176</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3544</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-D8F9-4031-9B78-DEFE5AA57454}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="13"/>
+          <c:tx>
+            <c:v>thujocci</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.0108440762908359E-2"/>
+                  <c:y val="0.28868997757081355"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$73:$A$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$73:$B$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4551</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2899</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3746</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2439</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000010-D8F9-4031-9B78-DEFE5AA57454}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2788,10 +3218,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4410E60-7558-47D7-A8E5-D3B5111C9A7A}">
-  <dimension ref="A1:V63"/>
+  <dimension ref="A1:V78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M28" workbookViewId="0">
-      <selection activeCell="S32" sqref="S32"/>
+    <sheetView tabSelected="1" topLeftCell="H16" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2867,7 +3297,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>5.0452036900000001</v>
+        <v>1.7943016941382393</v>
       </c>
       <c r="G4">
         <v>3000</v>
@@ -2887,7 +3317,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>125</v>
+        <v>200</v>
       </c>
       <c r="G5">
         <v>1500</v>
@@ -2921,7 +3351,7 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>7.0000000000000007E-2</v>
+        <v>0.08</v>
       </c>
       <c r="G7" t="s">
         <v>17</v>
@@ -2935,7 +3365,7 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>0.37</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -2943,7 +3373,7 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>4.1999999999999998E-5</v>
+        <v>8.2000000000000001E-5</v>
       </c>
       <c r="G9" t="s">
         <v>15</v>
@@ -2978,13 +3408,13 @@
       </c>
       <c r="B11">
         <f>LN(B5*B4*(1-B8)/(B1*B7))*(1-B8)*(-1/B9)</f>
-        <v>-15646.108240729833</v>
+        <v>-2988.2287748553731</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
       </c>
       <c r="D11">
-        <v>3252</v>
+        <v>2439</v>
       </c>
       <c r="G11">
         <v>2000</v>
@@ -3002,11 +3432,11 @@
       </c>
       <c r="B12">
         <f>B11/(1-$B8)</f>
-        <v>-24835.09244560291</v>
+        <v>-4597.275038239035</v>
       </c>
       <c r="D12">
         <f>D11/(1-$B8)</f>
-        <v>5161.9047619047615</v>
+        <v>3752.3076923076924</v>
       </c>
       <c r="G12">
         <v>3000</v>
@@ -3024,11 +3454,11 @@
       </c>
       <c r="B13">
         <f>EXP(-1*$B9*B12)</f>
-        <v>2.8379270756250006</v>
+        <v>1.4578701264873195</v>
       </c>
       <c r="D13">
         <f>EXP(-1*$B9*D12)</f>
-        <v>0.80509097139853514</v>
+        <v>0.73514374256895088</v>
       </c>
       <c r="G13">
         <v>1500</v>
@@ -3046,11 +3476,11 @@
       </c>
       <c r="B14">
         <f>B12*$B7*B13</f>
-        <v>-4933.612689391849</v>
+        <v>-536.17839531956315</v>
       </c>
       <c r="D14">
         <f>D12*$B7*D13</f>
-        <v>290.90620433200399</v>
+        <v>220.67884161546721</v>
       </c>
       <c r="G14" t="s">
         <v>16</v>
@@ -3062,11 +3492,11 @@
       </c>
       <c r="B15">
         <f>B14/$B5</f>
-        <v>-39.468901515134789</v>
+        <v>-2.6808919765978159</v>
       </c>
       <c r="D15">
         <f>(D$14/$B$3)/($B$5-$B$6*0*D$14/$B$3)</f>
-        <v>0.4654499269312064</v>
+        <v>0.22067884161546722</v>
       </c>
       <c r="G15" t="s">
         <v>17</v>
@@ -3078,16 +3508,16 @@
       </c>
       <c r="D16">
         <f>(D$14/$B$3)/($B$5-$B$6*1*D$14/$B$3)</f>
-        <v>0.4654499269312064</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+        <v>0.22067884161546722</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
       <c r="D17">
         <f>(D$14/$B$3)/($B$5-$B$6*2*D$14/$B$3)</f>
-        <v>0.4654499269312064</v>
+        <v>0.22067884161546722</v>
       </c>
       <c r="G17" t="s">
         <v>15</v>
@@ -3105,13 +3535,13 @@
         <v>6.2788776441618435</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
       <c r="D18">
         <f>(D$14/$B$3)/($B$5-$B$6*3*D$14/$B$3)</f>
-        <v>0.4654499269312064</v>
+        <v>0.22067884161546722</v>
       </c>
       <c r="G18">
         <v>4000</v>
@@ -3123,13 +3553,13 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>28</v>
       </c>
       <c r="D19">
         <f>(D$14/$B$3)/($B$5-$B$6*4*D$14/$B$3)</f>
-        <v>0.4654499269312064</v>
+        <v>0.22067884161546722</v>
       </c>
       <c r="G19">
         <v>2000</v>
@@ -3156,13 +3586,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>11</v>
       </c>
       <c r="D20">
         <f>SUM(D15:D19)</f>
-        <v>2.3272496346560319</v>
+        <v>1.103394208077336</v>
       </c>
       <c r="G20">
         <v>3000</v>
@@ -3194,17 +3624,17 @@
         <v>1528.6</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>12</v>
       </c>
       <c r="B21">
         <f>B15/$B4</f>
-        <v>-7.823054120364918</v>
+        <v>-1.4941143874276868</v>
       </c>
       <c r="D21">
         <f>D20/$B4</f>
-        <v>0.46127961875331774</v>
+        <v>0.61494352464916457</v>
       </c>
       <c r="G21">
         <v>1500</v>
@@ -3236,17 +3666,17 @@
         <v>1429.3</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>14</v>
       </c>
       <c r="B22">
         <f>B21*B11</f>
-        <v>122400.35154031702</v>
+        <v>4464.7556054368224</v>
       </c>
       <c r="D22">
         <f>D21*D11</f>
-        <v>1500.0813201857893</v>
+        <v>1499.8472566193125</v>
       </c>
       <c r="G22" t="s">
         <v>16</v>
@@ -3272,7 +3702,7 @@
         <v>2025.7</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G23" t="s">
         <v>17</v>
       </c>
@@ -3297,7 +3727,7 @@
         <v>1892.6</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -3334,7 +3764,7 @@
         <v>1365.6</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>4000</v>
       </c>
@@ -3383,7 +3813,7 @@
         <v>1766.3</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2000</v>
       </c>
@@ -3429,7 +3859,7 @@
         <v>1485.4</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>3000</v>
       </c>
@@ -3475,7 +3905,7 @@
         <v>1981.8</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1500</v>
       </c>
@@ -3521,7 +3951,7 @@
         <v>1890.5</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -3561,7 +3991,7 @@
         <v>1681.6</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -3595,15 +4025,38 @@
         <v>1784.9</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G31" t="s">
         <v>17</v>
       </c>
       <c r="H31">
         <v>1429.3</v>
       </c>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="M31" t="s">
+        <v>36</v>
+      </c>
+      <c r="N31">
+        <f>E69</f>
+        <v>0.33</v>
+      </c>
+      <c r="O31">
+        <f>E70</f>
+        <v>7.4999999999999993E-5</v>
+      </c>
+      <c r="P31">
+        <f>E68</f>
+        <v>0.11</v>
+      </c>
+      <c r="Q31">
+        <f>B69</f>
+        <v>1.3303</v>
+      </c>
+      <c r="R31">
+        <f>B70</f>
+        <v>1458.9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -3619,32 +4072,28 @@
       <c r="E32">
         <v>5</v>
       </c>
-      <c r="N32" t="s">
-        <v>20</v>
-      </c>
-      <c r="O32" t="s">
-        <v>19</v>
-      </c>
-      <c r="P32" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>5</v>
-      </c>
-      <c r="R32" t="s">
-        <v>3</v>
-      </c>
-      <c r="S32" t="s">
-        <v>21</v>
-      </c>
-      <c r="T32" t="s">
-        <v>31</v>
-      </c>
-      <c r="U32" t="s">
-        <v>32</v>
-      </c>
-      <c r="V32" t="s">
-        <v>33</v>
+      <c r="M32" t="s">
+        <v>41</v>
+      </c>
+      <c r="N32">
+        <f>K70</f>
+        <v>0.37</v>
+      </c>
+      <c r="O32">
+        <f>K71</f>
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="P32">
+        <f>K69</f>
+        <v>0.02</v>
+      </c>
+      <c r="Q32">
+        <f>H70</f>
+        <v>1.0163</v>
+      </c>
+      <c r="R32">
+        <f>H71</f>
+        <v>2070.6</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.3">
@@ -3675,29 +4124,28 @@
       <c r="K33" s="1">
         <v>3.1229154598594424</v>
       </c>
+      <c r="M33" t="s">
+        <v>42</v>
+      </c>
+      <c r="N33">
+        <f>E77</f>
+        <v>0.35</v>
+      </c>
       <c r="O33">
-        <v>-10.52111</v>
+        <f>E78</f>
+        <v>8.2000000000000001E-5</v>
       </c>
       <c r="P33">
-        <v>37.175379999999997</v>
+        <f>E76</f>
+        <v>0.08</v>
       </c>
       <c r="Q33">
-        <v>260587.60664000001</v>
+        <f>B77</f>
+        <v>0.84250000000000003</v>
       </c>
       <c r="R33">
-        <v>389.34181999999998</v>
-      </c>
-      <c r="S33">
-        <v>-860591.71869999997</v>
-      </c>
-      <c r="T33">
-        <v>-1254.4416699999999</v>
-      </c>
-      <c r="U33">
-        <v>-8818197.8019299991</v>
-      </c>
-      <c r="V33">
-        <v>28741687.899459999</v>
+        <f>B78</f>
+        <v>1197.3</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.3">
@@ -3751,33 +4199,6 @@
       <c r="K35">
         <v>0.03</v>
       </c>
-      <c r="N35" t="s">
-        <v>22</v>
-      </c>
-      <c r="O35" t="s">
-        <v>19</v>
-      </c>
-      <c r="P35" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>5</v>
-      </c>
-      <c r="R35" t="s">
-        <v>3</v>
-      </c>
-      <c r="S35" t="s">
-        <v>21</v>
-      </c>
-      <c r="T35" t="s">
-        <v>31</v>
-      </c>
-      <c r="U35" t="s">
-        <v>32</v>
-      </c>
-      <c r="V35" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36">
@@ -3804,29 +4225,32 @@
       <c r="K36">
         <v>0.28999999999999998</v>
       </c>
-      <c r="O36">
-        <v>3477.9259999999999</v>
-      </c>
-      <c r="P36">
-        <v>-4180.7430000000004</v>
-      </c>
-      <c r="Q36">
-        <v>-42869944.736000001</v>
-      </c>
-      <c r="R36">
-        <v>-4773.5860000000002</v>
-      </c>
-      <c r="S36">
-        <v>110938819.17</v>
-      </c>
-      <c r="T36">
-        <v>70594.072</v>
-      </c>
-      <c r="U36">
-        <v>671495174.11899996</v>
-      </c>
-      <c r="V36">
-        <v>-3252233432.9229999</v>
+      <c r="N36" t="s">
+        <v>20</v>
+      </c>
+      <c r="O36" t="s">
+        <v>19</v>
+      </c>
+      <c r="P36" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>5</v>
+      </c>
+      <c r="R36" t="s">
+        <v>3</v>
+      </c>
+      <c r="S36" t="s">
+        <v>21</v>
+      </c>
+      <c r="T36" t="s">
+        <v>31</v>
+      </c>
+      <c r="U36" t="s">
+        <v>32</v>
+      </c>
+      <c r="V36" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.3">
@@ -3854,6 +4278,30 @@
       <c r="K37" s="1">
         <v>3.8000000000000002E-5</v>
       </c>
+      <c r="O37">
+        <v>-8.2362850000000005</v>
+      </c>
+      <c r="P37">
+        <v>27.768424</v>
+      </c>
+      <c r="Q37">
+        <v>191053.281571</v>
+      </c>
+      <c r="R37">
+        <v>312.812679</v>
+      </c>
+      <c r="S37">
+        <v>-594492.21628399997</v>
+      </c>
+      <c r="T37">
+        <v>-941.44769499999995</v>
+      </c>
+      <c r="U37">
+        <v>-6490254.1347559998</v>
+      </c>
+      <c r="V37">
+        <v>19879995.810771</v>
+      </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
@@ -3883,25 +4331,31 @@
         <v>2025.7</v>
       </c>
       <c r="N39" t="s">
+        <v>22</v>
+      </c>
+      <c r="O39" t="s">
+        <v>19</v>
+      </c>
+      <c r="P39" t="s">
         <v>4</v>
       </c>
-      <c r="O39" t="s">
+      <c r="Q39" t="s">
         <v>5</v>
       </c>
-      <c r="P39" t="s">
+      <c r="R39" t="s">
         <v>3</v>
       </c>
-      <c r="Q39" t="s">
-        <v>16</v>
-      </c>
-      <c r="R39" t="s">
-        <v>19</v>
-      </c>
       <c r="S39" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="T39" t="s">
-        <v>6</v>
+        <v>31</v>
+      </c>
+      <c r="U39" t="s">
+        <v>32</v>
+      </c>
+      <c r="V39" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.3">
@@ -3920,29 +4374,29 @@
       <c r="E40">
         <v>5</v>
       </c>
-      <c r="N40">
-        <v>0.28999999999999998</v>
-      </c>
       <c r="O40">
-        <v>6.3E-5</v>
+        <v>1735.1790000000001</v>
       </c>
       <c r="P40">
-        <v>0.03</v>
+        <v>2994.393</v>
       </c>
       <c r="Q40">
-        <f>O$33+P$33*N40+Q$33*O40+S$33*N40*O40+P40*R$33+T$33*N40*P40+U$33*O40*P40+V$33*N40*O40*P40</f>
-        <v>0.80729608071733061</v>
+        <v>10167232.544</v>
       </c>
       <c r="R40">
-        <f>O$36+P$36*N40+Q$36*O40+S$36*N40*O40+R$36*P40+T$36*N40*P40+U$36*O40*P40+V$36*N40*O40*P40</f>
-        <v>1549.0938187677136</v>
+        <v>53598.870999999999</v>
       </c>
       <c r="S40">
-        <v>2000</v>
+        <v>-92028081.987000003</v>
       </c>
       <c r="T40">
-        <f>R40+S40*Q40</f>
-        <v>3163.6859802023746</v>
+        <v>-168141.49799999999</v>
+      </c>
+      <c r="U40">
+        <v>-1104139533.563</v>
+      </c>
+      <c r="V40">
+        <v>3507005746.0110002</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.3">
@@ -3973,30 +4427,6 @@
       <c r="K41" s="1">
         <v>3.1229154598594424</v>
       </c>
-      <c r="N41">
-        <v>0.37</v>
-      </c>
-      <c r="O41">
-        <v>4.3999999999999999E-5</v>
-      </c>
-      <c r="P41">
-        <v>0.03</v>
-      </c>
-      <c r="Q41">
-        <f t="shared" ref="Q41:Q44" si="0">O$33+P$33*N41+Q$33*O41+S$33*N41*O41+P41*R$33+T$33*N41*P41+U$33*O41*P41+V$33*N41*O41*P41</f>
-        <v>0.84257344627266662</v>
-      </c>
-      <c r="R41">
-        <f t="shared" ref="R41:R44" si="1">O$36+P$36*N41+Q$36*O41+S$36*N41*O41+R$36*P41+T$36*N41*P41+U$36*O41*P41+V$36*N41*O41*P41</f>
-        <v>1789.2269381010867</v>
-      </c>
-      <c r="S41">
-        <v>2000</v>
-      </c>
-      <c r="T41">
-        <f>R41+S41*Q41</f>
-        <v>3474.3738306464202</v>
-      </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A42">
@@ -4023,30 +4453,6 @@
       <c r="K42">
         <v>93</v>
       </c>
-      <c r="N42">
-        <v>0.37</v>
-      </c>
-      <c r="O42">
-        <v>4.3999999999999999E-5</v>
-      </c>
-      <c r="P42">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="Q42">
-        <f t="shared" si="0"/>
-        <v>1.0726304480956586</v>
-      </c>
-      <c r="R42">
-        <f t="shared" si="1"/>
-        <v>1696.7810986973168</v>
-      </c>
-      <c r="S42">
-        <v>2000</v>
-      </c>
-      <c r="T42">
-        <f>R42+S42*Q42</f>
-        <v>3842.0419948886338</v>
-      </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A43">
@@ -4073,32 +4479,29 @@
       <c r="K43">
         <v>0.03</v>
       </c>
-      <c r="M43" t="s">
-        <v>35</v>
-      </c>
-      <c r="N43">
-        <v>0.33</v>
-      </c>
-      <c r="O43">
-        <v>4.3999999999999999E-5</v>
-      </c>
-      <c r="P43">
-        <v>0.08</v>
-      </c>
-      <c r="Q43">
-        <f t="shared" si="0"/>
-        <v>1.093202249855139</v>
-      </c>
-      <c r="R43">
-        <f t="shared" si="1"/>
-        <v>1890.5001739799227</v>
-      </c>
-      <c r="S43">
-        <v>2000</v>
-      </c>
-      <c r="T43">
-        <f>R43+S43*Q43</f>
-        <v>4076.904673690201</v>
+      <c r="N43" t="s">
+        <v>4</v>
+      </c>
+      <c r="O43" t="s">
+        <v>5</v>
+      </c>
+      <c r="P43" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>1</v>
+      </c>
+      <c r="R43" t="s">
+        <v>16</v>
+      </c>
+      <c r="S43" t="s">
+        <v>19</v>
+      </c>
+      <c r="T43" t="s">
+        <v>23</v>
+      </c>
+      <c r="U43" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.3">
@@ -4126,32 +4529,29 @@
       <c r="K44" s="1">
         <v>0.37</v>
       </c>
-      <c r="M44" t="s">
-        <v>34</v>
-      </c>
       <c r="N44">
-        <v>0.37</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="O44">
-        <v>4.1999999999999998E-5</v>
+        <v>6.3E-5</v>
       </c>
       <c r="P44">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="Q44">
-        <f t="shared" si="0"/>
-        <v>0.90845947664039528</v>
+        <v>0.03</v>
       </c>
       <c r="R44">
-        <f t="shared" si="1"/>
-        <v>1785.1543893660205</v>
+        <f>O$37+P$37*N44+Q$37*O44+S$37*N44*O44+P44*R$37+T$37*N44*P44+U$37*O44*P44+V$37*N44*O44*P44</f>
+        <v>0.81497272015906574</v>
       </c>
       <c r="S44">
+        <f>O$40+P$40*N44+Q$40*O44+S$40*N44*O44+R$40*P44+T$40*N44*P44+U$40*O44*P44+V$40*N44*O44*P44</f>
+        <v>1543.2367907240696</v>
+      </c>
+      <c r="T44">
         <v>2000</v>
       </c>
-      <c r="T44">
-        <f>R44+S44*Q44</f>
-        <v>3602.0733426468109</v>
+      <c r="U44">
+        <f>S44+T44*R44</f>
+        <v>3173.1822310422012</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.3">
@@ -4179,6 +4579,30 @@
       <c r="K45" s="1">
         <v>3.8000000000000002E-5</v>
       </c>
+      <c r="N45">
+        <v>0.37</v>
+      </c>
+      <c r="O45">
+        <v>4.3999999999999999E-5</v>
+      </c>
+      <c r="P45">
+        <v>0.03</v>
+      </c>
+      <c r="R45">
+        <f>O$37+P$37*N45+Q$37*O45+S$37*N45*O45+P45*R$37+T$37*N45*P45+U$37*O45*P45+V$37*N45*O45*P45</f>
+        <v>0.84260843962311505</v>
+      </c>
+      <c r="S45">
+        <f>O$40+P$40*N45+Q$40*O45+S$40*N45*O45+R$40*P45+T$40*N45*P45+U$40*O45*P45+V$40*N45*O45*P45</f>
+        <v>1789.1983914362527</v>
+      </c>
+      <c r="T45">
+        <v>2000</v>
+      </c>
+      <c r="U45">
+        <f>S45+T45*R45</f>
+        <v>3474.4152706824825</v>
+      </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
@@ -4199,6 +4623,33 @@
       <c r="H46">
         <v>0.85440000000000005</v>
       </c>
+      <c r="M46" t="s">
+        <v>35</v>
+      </c>
+      <c r="N46">
+        <v>0.33</v>
+      </c>
+      <c r="O46">
+        <v>4.5000000000000003E-5</v>
+      </c>
+      <c r="P46">
+        <v>0.06</v>
+      </c>
+      <c r="R46">
+        <f>O$37+P$37*N46+Q$37*O46+S$37*N46*O46+P46*R$37+T$37*N46*P46+U$37*O46*P46+V$37*N46*O46*P46</f>
+        <v>1.0139696614333573</v>
+      </c>
+      <c r="S46">
+        <f>O$40+P$40*N46+Q$40*O46+S$40*N46*O46+R$40*P46+T$40*N46*P46+U$40*O46*P46+V$40*N46*O46*P46</f>
+        <v>1844.5331156487518</v>
+      </c>
+      <c r="T46">
+        <v>2000</v>
+      </c>
+      <c r="U46">
+        <f>S46+T46*R46</f>
+        <v>3872.4724385154664</v>
+      </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G47" t="s">
@@ -4207,6 +4658,33 @@
       <c r="H47">
         <v>1892.6</v>
       </c>
+      <c r="M47" t="s">
+        <v>34</v>
+      </c>
+      <c r="N47">
+        <v>0.33</v>
+      </c>
+      <c r="O47">
+        <v>4.3999999999999999E-5</v>
+      </c>
+      <c r="P47">
+        <v>0.08</v>
+      </c>
+      <c r="R47">
+        <f>O$37+P$37*N47+Q$37*O47+S$37*N47*O47+P47*R$37+T$37*N47*P47+U$37*O47*P47+V$37*N47*O47*P47</f>
+        <v>1.119316080130794</v>
+      </c>
+      <c r="S47">
+        <f>O$40+P$40*N47+Q$40*O47+S$40*N47*O47+R$40*P47+T$40*N47*P47+U$40*O47*P47+V$40*N47*O47*P47</f>
+        <v>1870.5800207093766</v>
+      </c>
+      <c r="T47">
+        <v>2000</v>
+      </c>
+      <c r="U47">
+        <f>S47+T47*R47</f>
+        <v>4109.2121809709643</v>
+      </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
@@ -4224,8 +4702,32 @@
       <c r="E48">
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N48">
+        <v>0.37</v>
+      </c>
+      <c r="O48">
+        <v>4.1999999999999998E-5</v>
+      </c>
+      <c r="P48">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R48">
+        <f>O$37+P$37*N48+Q$37*O48+S$37*N48*O48+P48*R$37+T$37*N48*P48+U$37*O48*P48+V$37*N48*O48*P48</f>
+        <v>0.88136518120268903</v>
+      </c>
+      <c r="S48">
+        <f>O$40+P$40*N48+Q$40*O48+S$40*N48*O48+R$40*P48+T$40*N48*P48+U$40*O48*P48+V$40*N48*O48*P48</f>
+        <v>1805.8185764055665</v>
+      </c>
+      <c r="T48">
+        <v>2000</v>
+      </c>
+      <c r="U48">
+        <f>S48+T48*R48</f>
+        <v>3568.5489388109445</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>4000</v>
       </c>
@@ -4253,8 +4755,35 @@
       <c r="K49">
         <v>5</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M49" t="s">
+        <v>36</v>
+      </c>
+      <c r="N49">
+        <v>0.33</v>
+      </c>
+      <c r="O49" s="3">
+        <v>7.4999999999999993E-5</v>
+      </c>
+      <c r="P49">
+        <v>0.11</v>
+      </c>
+      <c r="R49">
+        <f>O$37+P$37*N49+Q$37*O49+S$37*N49*O49+P49*R$37+T$37*N49*P49+U$37*O49*P49+V$37*N49*O49*P49</f>
+        <v>1.3561440293830529</v>
+      </c>
+      <c r="S49">
+        <f>O$40+P$40*N49+Q$40*O49+S$40*N49*O49+R$40*P49+T$40*N49*P49+U$40*O49*P49+V$40*N49*O49*P49</f>
+        <v>1439.187525841945</v>
+      </c>
+      <c r="T49">
+        <v>2000</v>
+      </c>
+      <c r="U49">
+        <f>S49+T49*R49</f>
+        <v>4151.4755846080507</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2000</v>
       </c>
@@ -4279,8 +4808,35 @@
       <c r="K50" s="1">
         <v>5.0452036900000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M50" t="s">
+        <v>37</v>
+      </c>
+      <c r="N50">
+        <v>0.37</v>
+      </c>
+      <c r="O50">
+        <v>4.1999999999999998E-5</v>
+      </c>
+      <c r="P50">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="R50">
+        <f>O$37+P$37*N50+Q$37*O50+S$37*N50*O50+P50*R$37+T$37*N50*P50+U$37*O50*P50+V$37*N50*O50*P50</f>
+        <v>0.88547264665083603</v>
+      </c>
+      <c r="S50">
+        <f>O$40+P$40*N50+Q$40*O50+S$40*N50*O50+R$40*P50+T$40*N50*P50+U$40*O50*P50+V$40*N50*O50*P50</f>
+        <v>1803.3762045223907</v>
+      </c>
+      <c r="T50">
+        <v>2000</v>
+      </c>
+      <c r="U50">
+        <f>S50+T50*R50</f>
+        <v>3574.321497824063</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>3000</v>
       </c>
@@ -4305,8 +4861,35 @@
       <c r="K51" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M51" t="s">
+        <v>38</v>
+      </c>
+      <c r="N51">
+        <v>0.31</v>
+      </c>
+      <c r="O51">
+        <v>5.7000000000000003E-5</v>
+      </c>
+      <c r="P51">
+        <v>2.7E-2</v>
+      </c>
+      <c r="R51">
+        <f>O$37+P$37*N51+Q$37*O51+S$37*N51*O51+P51*R$37+T$37*N51*P51+U$37*O51*P51+V$37*N51*O51*P51</f>
+        <v>0.81935724162997303</v>
+      </c>
+      <c r="S51">
+        <f>O$40+P$40*N51+Q$40*O51+S$40*N51*O51+R$40*P51+T$40*N51*P51+U$40*O51*P51+V$40*N51*O51*P51</f>
+        <v>1630.5486842486412</v>
+      </c>
+      <c r="T51">
+        <v>2000</v>
+      </c>
+      <c r="U51">
+        <f>S51+T51*R51</f>
+        <v>3269.2631675085872</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>1500</v>
       </c>
@@ -4331,8 +4914,35 @@
       <c r="K52" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M52" t="s">
+        <v>40</v>
+      </c>
+      <c r="N52">
+        <v>0.31</v>
+      </c>
+      <c r="O52">
+        <v>4.6999999999999997E-5</v>
+      </c>
+      <c r="P52">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="R52">
+        <f>O$37+P$37*N52+Q$37*O52+S$37*N52*O52+P52*R$37+T$37*N52*P52+U$37*O52*P52+V$37*N52*O52*P52</f>
+        <v>0.80672233434655283</v>
+      </c>
+      <c r="S52">
+        <f>O$40+P$40*N52+Q$40*O52+S$40*N52*O52+R$40*P52+T$40*N52*P52+U$40*O52*P52+V$40*N52*O52*P52</f>
+        <v>1814.6795725177149</v>
+      </c>
+      <c r="T52">
+        <v>2000</v>
+      </c>
+      <c r="U52">
+        <f t="shared" ref="U52:U53" si="0">S52+T52*R52</f>
+        <v>3428.1242412108204</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>16</v>
       </c>
@@ -4357,8 +4967,35 @@
       <c r="K53" s="1">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M53" t="s">
+        <v>39</v>
+      </c>
+      <c r="N53">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="O53">
+        <v>3.6999999999999998E-5</v>
+      </c>
+      <c r="P53">
+        <v>2.3E-2</v>
+      </c>
+      <c r="R53">
+        <f>O$37+P$37*N53+Q$37*O53+S$37*N53*O53+P53*R$37+T$37*N53*P53+U$37*O53*P53+V$37*N53*O53*P53</f>
+        <v>0.54045946711067872</v>
+      </c>
+      <c r="S53">
+        <f>O$40+P$40*N53+Q$40*O53+S$40*N53*O53+R$40*P53+T$40*N53*P53+U$40*O53*P53+V$40*N53*O53*P53</f>
+        <v>2359.2475431476596</v>
+      </c>
+      <c r="T53">
+        <v>2000</v>
+      </c>
+      <c r="U53">
+        <f t="shared" si="0"/>
+        <v>3440.1664773690172</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>17</v>
       </c>
@@ -4383,8 +5020,38 @@
       <c r="K54" s="1">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M54" t="s">
+        <v>41</v>
+      </c>
+      <c r="N54">
+        <v>0.35</v>
+      </c>
+      <c r="O54">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="P54">
+        <v>0.02</v>
+      </c>
+      <c r="Q54">
+        <v>3.1469580000000001</v>
+      </c>
+      <c r="R54">
+        <f>O$37+P$37*N54+Q$37*O54+S$37*N54*O54+P54*R$37+T$37*N54*P54+U$37*O54*P54+V$37*N54*O54*P54</f>
+        <v>0.84221886907508114</v>
+      </c>
+      <c r="S54">
+        <f>O$40+P$40*N54+Q$40*O54+S$40*N54*O54+R$40*P54+T$40*N54*P54+U$40*O54*P54+V$40*N54*O54*P54</f>
+        <v>1895.1496199746798</v>
+      </c>
+      <c r="T54">
+        <v>2000</v>
+      </c>
+      <c r="U54">
+        <f t="shared" ref="U54:U55" si="1">S54+T54*R54</f>
+        <v>3579.587358124842</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
       <c r="G55" t="s">
         <v>17</v>
       </c>
@@ -4397,8 +5064,38 @@
       <c r="K55" s="1">
         <v>4.1999999999999998E-5</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M55" t="s">
+        <v>42</v>
+      </c>
+      <c r="N55">
+        <v>0.35</v>
+      </c>
+      <c r="O55">
+        <v>8.2000000000000001E-5</v>
+      </c>
+      <c r="P55">
+        <v>0.08</v>
+      </c>
+      <c r="Q55">
+        <v>1.7943016941382393</v>
+      </c>
+      <c r="R55">
+        <f>O$37+P$37*N55+Q$37*O55+S$37*N55*O55+P55*R$37+T$37*N55*P55+U$37*O55*P55+V$37*N55*O55*P55</f>
+        <v>1.8199879990020591</v>
+      </c>
+      <c r="S55">
+        <f>O$40+P$40*N55+Q$40*O55+S$40*N55*O55+R$40*P55+T$40*N55*P55+U$40*O55*P55+V$40*N55*O55*P55</f>
+        <v>1364.6012542490762</v>
+      </c>
+      <c r="T55">
+        <v>2000</v>
+      </c>
+      <c r="U55">
+        <f t="shared" si="1"/>
+        <v>5004.5772522531943</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>15</v>
       </c>
@@ -4415,7 +5112,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>4000</v>
       </c>
@@ -4444,7 +5141,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2000</v>
       </c>
@@ -4470,7 +5167,7 @@
         <v>5.0452036900000001</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>3000</v>
       </c>
@@ -4496,7 +5193,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>1500</v>
       </c>
@@ -4522,7 +5219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>16</v>
       </c>
@@ -4548,7 +5245,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>17</v>
       </c>
@@ -4574,7 +5271,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="G63" t="s">
         <v>17</v>
       </c>
@@ -4586,6 +5283,297 @@
       </c>
       <c r="K63" s="1">
         <v>4.1999999999999998E-5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>15</v>
+      </c>
+      <c r="B64" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64" t="s">
+        <v>30</v>
+      </c>
+      <c r="E64">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>4000</v>
+      </c>
+      <c r="B65">
+        <v>6778</v>
+      </c>
+      <c r="D65" t="s">
+        <v>1</v>
+      </c>
+      <c r="E65" s="1">
+        <v>5.2868905100000001</v>
+      </c>
+      <c r="G65" t="s">
+        <v>15</v>
+      </c>
+      <c r="H65" t="s">
+        <v>6</v>
+      </c>
+      <c r="I65" t="s">
+        <v>9</v>
+      </c>
+      <c r="J65" t="s">
+        <v>30</v>
+      </c>
+      <c r="K65">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>2000</v>
+      </c>
+      <c r="B66">
+        <v>4133</v>
+      </c>
+      <c r="D66" t="s">
+        <v>2</v>
+      </c>
+      <c r="E66" s="1">
+        <v>167</v>
+      </c>
+      <c r="G66">
+        <v>4000</v>
+      </c>
+      <c r="H66">
+        <v>6095</v>
+      </c>
+      <c r="J66" t="s">
+        <v>1</v>
+      </c>
+      <c r="K66" s="1">
+        <v>3.1469580000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>3000</v>
+      </c>
+      <c r="B67">
+        <v>5449</v>
+      </c>
+      <c r="D67" t="s">
+        <v>29</v>
+      </c>
+      <c r="E67" s="1">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>2000</v>
+      </c>
+      <c r="H67">
+        <v>4139</v>
+      </c>
+      <c r="J67" t="s">
+        <v>2</v>
+      </c>
+      <c r="K67" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>1500</v>
+      </c>
+      <c r="B68">
+        <v>3444</v>
+      </c>
+      <c r="D68" t="s">
+        <v>3</v>
+      </c>
+      <c r="E68" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="G68">
+        <v>3000</v>
+      </c>
+      <c r="H68">
+        <v>5176</v>
+      </c>
+      <c r="J68" t="s">
+        <v>29</v>
+      </c>
+      <c r="K68" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>16</v>
+      </c>
+      <c r="B69">
+        <v>1.3303</v>
+      </c>
+      <c r="D69" t="s">
+        <v>4</v>
+      </c>
+      <c r="E69" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="G69">
+        <v>1500</v>
+      </c>
+      <c r="H69">
+        <v>3544</v>
+      </c>
+      <c r="J69" t="s">
+        <v>3</v>
+      </c>
+      <c r="K69" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>17</v>
+      </c>
+      <c r="B70">
+        <v>1458.9</v>
+      </c>
+      <c r="D70" t="s">
+        <v>5</v>
+      </c>
+      <c r="E70" s="1">
+        <v>7.4999999999999993E-5</v>
+      </c>
+      <c r="G70" t="s">
+        <v>16</v>
+      </c>
+      <c r="H70">
+        <v>1.0163</v>
+      </c>
+      <c r="J70" t="s">
+        <v>4</v>
+      </c>
+      <c r="K70" s="1">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G71" t="s">
+        <v>17</v>
+      </c>
+      <c r="H71">
+        <v>2070.6</v>
+      </c>
+      <c r="J71" t="s">
+        <v>5</v>
+      </c>
+      <c r="K71" s="1">
+        <v>4.0000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>15</v>
+      </c>
+      <c r="B72" t="s">
+        <v>6</v>
+      </c>
+      <c r="C72" t="s">
+        <v>9</v>
+      </c>
+      <c r="D72" t="s">
+        <v>30</v>
+      </c>
+      <c r="E72">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>4000</v>
+      </c>
+      <c r="B73">
+        <v>4551</v>
+      </c>
+      <c r="D73" t="s">
+        <v>1</v>
+      </c>
+      <c r="E73" s="1">
+        <v>1.7943016941382393</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>2000</v>
+      </c>
+      <c r="B74">
+        <v>2899</v>
+      </c>
+      <c r="D74" t="s">
+        <v>2</v>
+      </c>
+      <c r="E74" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>3000</v>
+      </c>
+      <c r="B75">
+        <v>3746</v>
+      </c>
+      <c r="D75" t="s">
+        <v>29</v>
+      </c>
+      <c r="E75" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>1500</v>
+      </c>
+      <c r="B76">
+        <v>2439</v>
+      </c>
+      <c r="D76" t="s">
+        <v>3</v>
+      </c>
+      <c r="E76" s="1">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>16</v>
+      </c>
+      <c r="B77">
+        <v>0.84250000000000003</v>
+      </c>
+      <c r="D77" t="s">
+        <v>4</v>
+      </c>
+      <c r="E77" s="1">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>17</v>
+      </c>
+      <c r="B78">
+        <v>1197.3</v>
+      </c>
+      <c r="D78" t="s">
+        <v>5</v>
+      </c>
+      <c r="E78" s="1">
+        <v>8.2000000000000001E-5</v>
       </c>
     </row>
   </sheetData>
@@ -4596,10 +5584,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{808A42D6-C578-4F6D-A55C-60DFBA9F96D0}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4813,6 +5801,57 @@
         <v>1784.9</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0.33</v>
+      </c>
+      <c r="B13">
+        <v>7.4999999999999993E-5</v>
+      </c>
+      <c r="C13">
+        <v>0.11</v>
+      </c>
+      <c r="D13">
+        <v>1.3303</v>
+      </c>
+      <c r="E13">
+        <v>1458.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0.37</v>
+      </c>
+      <c r="B14">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="C14">
+        <v>0.02</v>
+      </c>
+      <c r="D14">
+        <v>1.0163</v>
+      </c>
+      <c r="E14">
+        <v>2070.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0.35</v>
+      </c>
+      <c r="B15">
+        <v>8.2000000000000001E-5</v>
+      </c>
+      <c r="C15">
+        <v>0.08</v>
+      </c>
+      <c r="D15">
+        <v>0.84250000000000003</v>
+      </c>
+      <c r="E15">
+        <v>1197.3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>